<commit_message>
Importing campaign spreadsheet works
</commit_message>
<xml_diff>
--- a/333 Project/Spreadsheets/5eClassSpells.xlsx
+++ b/333 Project/Spreadsheets/5eClassSpells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansarij\Documents\333 Classwork\Project\Git\333 Project\Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EE1BE3-8794-4BCF-9A84-604E3755ADBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261F2437-F3F5-4DCC-99DE-47A75B01BC6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1956" yWindow="2484" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17292" windowHeight="9420" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bard Spells" sheetId="2" r:id="rId1"/>
@@ -3265,10 +3265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A1277"/>
+  <dimension ref="A1:A750"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AC1"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5765,1589 +5765,8 @@
     <row r="749" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A749" s="3"/>
     </row>
-    <row r="750" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A750" s="3"/>
-    </row>
-    <row r="751" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A751" s="3"/>
-    </row>
-    <row r="752" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A752" s="3"/>
-    </row>
-    <row r="753" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A753" s="3"/>
-    </row>
-    <row r="754" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A754" s="3"/>
-    </row>
-    <row r="755" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A755" s="3"/>
-    </row>
-    <row r="756" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A756" s="3"/>
-    </row>
-    <row r="757" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A757" s="3"/>
-    </row>
-    <row r="758" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A758" s="3"/>
-    </row>
-    <row r="759" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A759" s="3"/>
-    </row>
-    <row r="760" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A760" s="3"/>
-    </row>
-    <row r="761" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A761" s="3"/>
-    </row>
-    <row r="762" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A762" s="3"/>
-    </row>
-    <row r="763" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A763" s="3"/>
-    </row>
-    <row r="764" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A764" s="3"/>
-    </row>
-    <row r="765" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A765" s="3"/>
-    </row>
-    <row r="766" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A766" s="3"/>
-    </row>
-    <row r="767" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A767" s="3"/>
-    </row>
-    <row r="768" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A768" s="3"/>
-    </row>
-    <row r="769" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A769" s="3"/>
-    </row>
-    <row r="770" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A770" s="3"/>
-    </row>
-    <row r="771" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A771" s="3"/>
-    </row>
-    <row r="772" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A772" s="3"/>
-    </row>
-    <row r="773" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A773" s="3"/>
-    </row>
-    <row r="774" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A774" s="3"/>
-    </row>
-    <row r="775" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A775" s="3"/>
-    </row>
-    <row r="776" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A776" s="3"/>
-    </row>
-    <row r="777" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A777" s="3"/>
-    </row>
-    <row r="778" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A778" s="3"/>
-    </row>
-    <row r="779" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A779" s="3"/>
-    </row>
-    <row r="780" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A780" s="3"/>
-    </row>
-    <row r="781" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A781" s="3"/>
-    </row>
-    <row r="782" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A782" s="3"/>
-    </row>
-    <row r="783" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A783" s="3"/>
-    </row>
-    <row r="784" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A784" s="3"/>
-    </row>
-    <row r="785" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A785" s="3"/>
-    </row>
-    <row r="786" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A786" s="3"/>
-    </row>
-    <row r="787" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A787" s="3"/>
-    </row>
-    <row r="788" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A788" s="3"/>
-    </row>
-    <row r="789" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A789" s="3"/>
-    </row>
-    <row r="790" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A790" s="3"/>
-    </row>
-    <row r="791" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A791" s="3"/>
-    </row>
-    <row r="792" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A792" s="3"/>
-    </row>
-    <row r="793" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A793" s="3"/>
-    </row>
-    <row r="794" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A794" s="3"/>
-    </row>
-    <row r="795" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A795" s="3"/>
-    </row>
-    <row r="796" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A796" s="3"/>
-    </row>
-    <row r="797" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A797" s="3"/>
-    </row>
-    <row r="798" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A798" s="3"/>
-    </row>
-    <row r="799" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A799" s="3"/>
-    </row>
-    <row r="800" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A800" s="3"/>
-    </row>
-    <row r="801" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A801" s="3"/>
-    </row>
-    <row r="802" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A802" s="3"/>
-    </row>
-    <row r="803" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A803" s="3"/>
-    </row>
-    <row r="804" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A804" s="3"/>
-    </row>
-    <row r="805" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A805" s="3"/>
-    </row>
-    <row r="806" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A806" s="3"/>
-    </row>
-    <row r="807" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A807" s="3"/>
-    </row>
-    <row r="808" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A808" s="3"/>
-    </row>
-    <row r="809" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A809" s="3"/>
-    </row>
-    <row r="810" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A810" s="3"/>
-    </row>
-    <row r="811" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A811" s="3"/>
-    </row>
-    <row r="812" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A812" s="3"/>
-    </row>
-    <row r="813" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A813" s="3"/>
-    </row>
-    <row r="814" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A814" s="3"/>
-    </row>
-    <row r="815" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A815" s="3"/>
-    </row>
-    <row r="816" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A816" s="3"/>
-    </row>
-    <row r="817" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A817" s="3"/>
-    </row>
-    <row r="818" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A818" s="3"/>
-    </row>
-    <row r="819" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A819" s="3"/>
-    </row>
-    <row r="820" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A820" s="3"/>
-    </row>
-    <row r="821" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A821" s="3"/>
-    </row>
-    <row r="822" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A822" s="3"/>
-    </row>
-    <row r="823" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A823" s="3"/>
-    </row>
-    <row r="824" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A824" s="3"/>
-    </row>
-    <row r="825" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A825" s="3"/>
-    </row>
-    <row r="826" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A826" s="3"/>
-    </row>
-    <row r="827" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A827" s="3"/>
-    </row>
-    <row r="828" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A828" s="3"/>
-    </row>
-    <row r="829" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A829" s="3"/>
-    </row>
-    <row r="830" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A830" s="3"/>
-    </row>
-    <row r="831" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A831" s="3"/>
-    </row>
-    <row r="832" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A832" s="3"/>
-    </row>
-    <row r="833" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A833" s="3"/>
-    </row>
-    <row r="834" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A834" s="3"/>
-    </row>
-    <row r="835" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A835" s="3"/>
-    </row>
-    <row r="836" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A836" s="3"/>
-    </row>
-    <row r="837" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A837" s="3"/>
-    </row>
-    <row r="838" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A838" s="3"/>
-    </row>
-    <row r="839" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A839" s="3"/>
-    </row>
-    <row r="840" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A840" s="3"/>
-    </row>
-    <row r="841" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A841" s="3"/>
-    </row>
-    <row r="842" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A842" s="3"/>
-    </row>
-    <row r="843" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A843" s="3"/>
-    </row>
-    <row r="844" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A844" s="3"/>
-    </row>
-    <row r="845" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A845" s="3"/>
-    </row>
-    <row r="846" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A846" s="3"/>
-    </row>
-    <row r="847" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A847" s="3"/>
-    </row>
-    <row r="848" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A848" s="3"/>
-    </row>
-    <row r="849" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A849" s="3"/>
-    </row>
-    <row r="850" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A850" s="3"/>
-    </row>
-    <row r="851" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A851" s="3"/>
-    </row>
-    <row r="852" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A852" s="3"/>
-    </row>
-    <row r="853" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A853" s="3"/>
-    </row>
-    <row r="854" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A854" s="3"/>
-    </row>
-    <row r="855" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A855" s="3"/>
-    </row>
-    <row r="856" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A856" s="3"/>
-    </row>
-    <row r="857" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A857" s="3"/>
-    </row>
-    <row r="858" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A858" s="3"/>
-    </row>
-    <row r="859" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A859" s="3"/>
-    </row>
-    <row r="860" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A860" s="3"/>
-    </row>
-    <row r="861" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A861" s="3"/>
-    </row>
-    <row r="862" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A862" s="3"/>
-    </row>
-    <row r="863" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A863" s="3"/>
-    </row>
-    <row r="864" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A864" s="3"/>
-    </row>
-    <row r="865" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A865" s="3"/>
-    </row>
-    <row r="866" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A866" s="3"/>
-    </row>
-    <row r="867" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A867" s="3"/>
-    </row>
-    <row r="868" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A868" s="3"/>
-    </row>
-    <row r="869" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A869" s="3"/>
-    </row>
-    <row r="870" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A870" s="3"/>
-    </row>
-    <row r="871" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A871" s="3"/>
-    </row>
-    <row r="872" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A872" s="3"/>
-    </row>
-    <row r="873" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A873" s="3"/>
-    </row>
-    <row r="874" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A874" s="3"/>
-    </row>
-    <row r="875" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A875" s="3"/>
-    </row>
-    <row r="876" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A876" s="3"/>
-    </row>
-    <row r="877" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A877" s="3"/>
-    </row>
-    <row r="878" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A878" s="3"/>
-    </row>
-    <row r="879" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A879" s="3"/>
-    </row>
-    <row r="880" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A880" s="3"/>
-    </row>
-    <row r="881" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A881" s="3"/>
-    </row>
-    <row r="882" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A882" s="3"/>
-    </row>
-    <row r="883" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A883" s="3"/>
-    </row>
-    <row r="884" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A884" s="3"/>
-    </row>
-    <row r="885" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A885" s="3"/>
-    </row>
-    <row r="886" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A886" s="3"/>
-    </row>
-    <row r="887" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A887" s="3"/>
-    </row>
-    <row r="888" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A888" s="3"/>
-    </row>
-    <row r="889" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A889" s="3"/>
-    </row>
-    <row r="890" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A890" s="3"/>
-    </row>
-    <row r="891" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A891" s="3"/>
-    </row>
-    <row r="892" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A892" s="3"/>
-    </row>
-    <row r="893" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A893" s="3"/>
-    </row>
-    <row r="894" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A894" s="3"/>
-    </row>
-    <row r="895" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A895" s="3"/>
-    </row>
-    <row r="896" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A896" s="3"/>
-    </row>
-    <row r="897" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A897" s="3"/>
-    </row>
-    <row r="898" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A898" s="3"/>
-    </row>
-    <row r="899" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A899" s="3"/>
-    </row>
-    <row r="900" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A900" s="3"/>
-    </row>
-    <row r="901" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A901" s="3"/>
-    </row>
-    <row r="902" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A902" s="3"/>
-    </row>
-    <row r="903" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A903" s="3"/>
-    </row>
-    <row r="904" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A904" s="3"/>
-    </row>
-    <row r="905" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A905" s="3"/>
-    </row>
-    <row r="906" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A906" s="3"/>
-    </row>
-    <row r="907" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A907" s="3"/>
-    </row>
-    <row r="908" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A908" s="3"/>
-    </row>
-    <row r="909" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A909" s="3"/>
-    </row>
-    <row r="910" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A910" s="3"/>
-    </row>
-    <row r="911" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A911" s="3"/>
-    </row>
-    <row r="912" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A912" s="3"/>
-    </row>
-    <row r="913" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A913" s="3"/>
-    </row>
-    <row r="914" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A914" s="3"/>
-    </row>
-    <row r="915" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A915" s="3"/>
-    </row>
-    <row r="916" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A916" s="3"/>
-    </row>
-    <row r="917" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A917" s="3"/>
-    </row>
-    <row r="918" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A918" s="3"/>
-    </row>
-    <row r="919" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A919" s="3"/>
-    </row>
-    <row r="920" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A920" s="3"/>
-    </row>
-    <row r="921" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A921" s="3"/>
-    </row>
-    <row r="922" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A922" s="3"/>
-    </row>
-    <row r="923" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A923" s="3"/>
-    </row>
-    <row r="924" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A924" s="3"/>
-    </row>
-    <row r="925" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A925" s="3"/>
-    </row>
-    <row r="926" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A926" s="3"/>
-    </row>
-    <row r="927" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A927" s="3"/>
-    </row>
-    <row r="928" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A928" s="3"/>
-    </row>
-    <row r="929" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A929" s="3"/>
-    </row>
-    <row r="930" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A930" s="3"/>
-    </row>
-    <row r="931" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A931" s="3"/>
-    </row>
-    <row r="932" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A932" s="3"/>
-    </row>
-    <row r="933" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A933" s="3"/>
-    </row>
-    <row r="934" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A934" s="3"/>
-    </row>
-    <row r="935" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A935" s="3"/>
-    </row>
-    <row r="936" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A936" s="3"/>
-    </row>
-    <row r="937" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A937" s="3"/>
-    </row>
-    <row r="938" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A938" s="3"/>
-    </row>
-    <row r="939" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A939" s="3"/>
-    </row>
-    <row r="940" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A940" s="3"/>
-    </row>
-    <row r="941" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A941" s="3"/>
-    </row>
-    <row r="942" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A942" s="3"/>
-    </row>
-    <row r="943" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A943" s="3"/>
-    </row>
-    <row r="944" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A944" s="3"/>
-    </row>
-    <row r="945" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A945" s="3"/>
-    </row>
-    <row r="946" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A946" s="3"/>
-    </row>
-    <row r="947" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A947" s="3"/>
-    </row>
-    <row r="948" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A948" s="3"/>
-    </row>
-    <row r="949" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A949" s="3"/>
-    </row>
-    <row r="950" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A950" s="3"/>
-    </row>
-    <row r="951" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A951" s="3"/>
-    </row>
-    <row r="952" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A952" s="3"/>
-    </row>
-    <row r="953" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A953" s="3"/>
-    </row>
-    <row r="954" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A954" s="3"/>
-    </row>
-    <row r="955" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A955" s="3"/>
-    </row>
-    <row r="956" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A956" s="3"/>
-    </row>
-    <row r="957" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A957" s="3"/>
-    </row>
-    <row r="958" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A958" s="3"/>
-    </row>
-    <row r="959" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A959" s="3"/>
-    </row>
-    <row r="960" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A960" s="3"/>
-    </row>
-    <row r="961" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A961" s="3"/>
-    </row>
-    <row r="962" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A962" s="3"/>
-    </row>
-    <row r="963" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A963" s="3"/>
-    </row>
-    <row r="964" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A964" s="3"/>
-    </row>
-    <row r="965" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A965" s="3"/>
-    </row>
-    <row r="966" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A966" s="3"/>
-    </row>
-    <row r="967" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A967" s="3"/>
-    </row>
-    <row r="968" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A968" s="3"/>
-    </row>
-    <row r="969" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A969" s="3"/>
-    </row>
-    <row r="970" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A970" s="3"/>
-    </row>
-    <row r="971" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A971" s="3"/>
-    </row>
-    <row r="972" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A972" s="3"/>
-    </row>
-    <row r="973" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A973" s="3"/>
-    </row>
-    <row r="974" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A974" s="3"/>
-    </row>
-    <row r="975" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A975" s="3"/>
-    </row>
-    <row r="976" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A976" s="3"/>
-    </row>
-    <row r="977" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A977" s="3"/>
-    </row>
-    <row r="978" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A978" s="3"/>
-    </row>
-    <row r="979" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A979" s="3"/>
-    </row>
-    <row r="980" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A980" s="3"/>
-    </row>
-    <row r="981" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A981" s="3"/>
-    </row>
-    <row r="982" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A982" s="3"/>
-    </row>
-    <row r="983" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A983" s="3"/>
-    </row>
-    <row r="984" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A984" s="3"/>
-    </row>
-    <row r="985" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A985" s="3"/>
-    </row>
-    <row r="986" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A986" s="3"/>
-    </row>
-    <row r="987" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A987" s="3"/>
-    </row>
-    <row r="988" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A988" s="3"/>
-    </row>
-    <row r="989" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A989" s="3"/>
-    </row>
-    <row r="990" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A990" s="3"/>
-    </row>
-    <row r="991" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A991" s="3"/>
-    </row>
-    <row r="992" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A992" s="3"/>
-    </row>
-    <row r="993" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A993" s="3"/>
-    </row>
-    <row r="994" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A994" s="3"/>
-    </row>
-    <row r="995" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A995" s="3"/>
-    </row>
-    <row r="996" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A996" s="3"/>
-    </row>
-    <row r="997" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A997" s="3"/>
-    </row>
-    <row r="998" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A998" s="3"/>
-    </row>
-    <row r="999" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A999" s="3"/>
-    </row>
-    <row r="1000" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1000" s="3"/>
-    </row>
-    <row r="1001" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1001" s="3"/>
-    </row>
-    <row r="1002" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1002" s="3"/>
-    </row>
-    <row r="1003" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1003" s="3"/>
-    </row>
-    <row r="1004" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1004" s="3"/>
-    </row>
-    <row r="1005" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1005" s="3"/>
-    </row>
-    <row r="1006" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1006" s="3"/>
-    </row>
-    <row r="1007" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1007" s="3"/>
-    </row>
-    <row r="1008" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1008" s="3"/>
-    </row>
-    <row r="1009" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1009" s="3"/>
-    </row>
-    <row r="1010" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1010" s="3"/>
-    </row>
-    <row r="1011" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1011" s="3"/>
-    </row>
-    <row r="1012" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1012" s="3"/>
-    </row>
-    <row r="1013" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1013" s="3"/>
-    </row>
-    <row r="1014" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1014" s="3"/>
-    </row>
-    <row r="1015" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1015" s="3"/>
-    </row>
-    <row r="1016" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1016" s="3"/>
-    </row>
-    <row r="1017" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1017" s="3"/>
-    </row>
-    <row r="1018" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1018" s="3"/>
-    </row>
-    <row r="1019" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1019" s="3"/>
-    </row>
-    <row r="1020" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1020" s="3"/>
-    </row>
-    <row r="1021" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1021" s="3"/>
-    </row>
-    <row r="1022" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1022" s="3"/>
-    </row>
-    <row r="1023" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1023" s="3"/>
-    </row>
-    <row r="1024" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1024" s="3"/>
-    </row>
-    <row r="1025" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1025" s="3"/>
-    </row>
-    <row r="1026" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1026" s="3"/>
-    </row>
-    <row r="1027" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1027" s="3"/>
-    </row>
-    <row r="1028" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1028" s="3"/>
-    </row>
-    <row r="1029" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1029" s="3"/>
-    </row>
-    <row r="1030" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1030" s="3"/>
-    </row>
-    <row r="1031" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1031" s="3"/>
-    </row>
-    <row r="1032" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1032" s="3"/>
-    </row>
-    <row r="1033" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1033" s="3"/>
-    </row>
-    <row r="1034" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1034" s="3"/>
-    </row>
-    <row r="1035" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1035" s="3"/>
-    </row>
-    <row r="1036" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1036" s="3"/>
-    </row>
-    <row r="1037" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1037" s="3"/>
-    </row>
-    <row r="1038" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1038" s="3"/>
-    </row>
-    <row r="1039" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1039" s="3"/>
-    </row>
-    <row r="1040" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1040" s="3"/>
-    </row>
-    <row r="1041" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1041" s="3"/>
-    </row>
-    <row r="1042" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1042" s="3"/>
-    </row>
-    <row r="1043" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1043" s="3"/>
-    </row>
-    <row r="1044" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1044" s="3"/>
-    </row>
-    <row r="1045" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1045" s="3"/>
-    </row>
-    <row r="1046" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1046" s="3"/>
-    </row>
-    <row r="1047" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1047" s="3"/>
-    </row>
-    <row r="1048" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1048" s="3"/>
-    </row>
-    <row r="1049" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1049" s="3"/>
-    </row>
-    <row r="1050" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1050" s="3"/>
-    </row>
-    <row r="1051" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1051" s="3"/>
-    </row>
-    <row r="1052" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1052" s="3"/>
-    </row>
-    <row r="1053" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1053" s="3"/>
-    </row>
-    <row r="1054" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1054" s="3"/>
-    </row>
-    <row r="1055" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1055" s="3"/>
-    </row>
-    <row r="1056" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1056" s="3"/>
-    </row>
-    <row r="1057" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1057" s="3"/>
-    </row>
-    <row r="1058" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1058" s="3"/>
-    </row>
-    <row r="1059" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1059" s="3"/>
-    </row>
-    <row r="1060" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1060" s="3"/>
-    </row>
-    <row r="1061" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1061" s="3"/>
-    </row>
-    <row r="1062" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1062" s="3"/>
-    </row>
-    <row r="1063" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1063" s="3"/>
-    </row>
-    <row r="1064" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1064" s="3"/>
-    </row>
-    <row r="1065" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1065" s="3"/>
-    </row>
-    <row r="1066" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1066" s="3"/>
-    </row>
-    <row r="1067" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1067" s="3"/>
-    </row>
-    <row r="1068" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1068" s="3"/>
-    </row>
-    <row r="1069" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1069" s="3"/>
-    </row>
-    <row r="1070" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1070" s="3"/>
-    </row>
-    <row r="1071" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1071" s="3"/>
-    </row>
-    <row r="1072" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1072" s="3"/>
-    </row>
-    <row r="1073" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1073" s="3"/>
-    </row>
-    <row r="1074" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1074" s="3"/>
-    </row>
-    <row r="1075" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1075" s="3"/>
-    </row>
-    <row r="1076" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1076" s="3"/>
-    </row>
-    <row r="1077" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1077" s="3"/>
-    </row>
-    <row r="1078" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1078" s="3"/>
-    </row>
-    <row r="1079" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1079" s="3"/>
-    </row>
-    <row r="1080" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1080" s="3"/>
-    </row>
-    <row r="1081" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1081" s="3"/>
-    </row>
-    <row r="1082" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1082" s="3"/>
-    </row>
-    <row r="1083" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1083" s="3"/>
-    </row>
-    <row r="1084" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1084" s="3"/>
-    </row>
-    <row r="1085" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1085" s="3"/>
-    </row>
-    <row r="1086" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1086" s="3"/>
-    </row>
-    <row r="1087" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1087" s="3"/>
-    </row>
-    <row r="1088" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1088" s="3"/>
-    </row>
-    <row r="1089" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1089" s="3"/>
-    </row>
-    <row r="1090" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1090" s="3"/>
-    </row>
-    <row r="1091" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1091" s="3"/>
-    </row>
-    <row r="1092" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1092" s="3"/>
-    </row>
-    <row r="1093" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1093" s="3"/>
-    </row>
-    <row r="1094" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1094" s="3"/>
-    </row>
-    <row r="1095" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1095" s="3"/>
-    </row>
-    <row r="1096" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1096" s="3"/>
-    </row>
-    <row r="1097" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1097" s="3"/>
-    </row>
-    <row r="1098" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1098" s="3"/>
-    </row>
-    <row r="1099" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1099" s="3"/>
-    </row>
-    <row r="1100" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1100" s="3"/>
-    </row>
-    <row r="1101" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1101" s="3"/>
-    </row>
-    <row r="1102" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1102" s="3"/>
-    </row>
-    <row r="1103" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1103" s="3"/>
-    </row>
-    <row r="1104" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1104" s="3"/>
-    </row>
-    <row r="1105" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1105" s="3"/>
-    </row>
-    <row r="1106" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1106" s="3"/>
-    </row>
-    <row r="1107" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1107" s="3"/>
-    </row>
-    <row r="1108" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1108" s="3"/>
-    </row>
-    <row r="1109" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1109" s="3"/>
-    </row>
-    <row r="1110" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1110" s="3"/>
-    </row>
-    <row r="1111" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1111" s="3"/>
-    </row>
-    <row r="1112" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1112" s="3"/>
-    </row>
-    <row r="1113" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1113" s="3"/>
-    </row>
-    <row r="1114" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1114" s="3"/>
-    </row>
-    <row r="1115" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1115" s="3"/>
-    </row>
-    <row r="1116" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1116" s="3"/>
-    </row>
-    <row r="1117" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1117" s="3"/>
-    </row>
-    <row r="1118" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1118" s="3"/>
-    </row>
-    <row r="1119" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1119" s="3"/>
-    </row>
-    <row r="1120" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1120" s="3"/>
-    </row>
-    <row r="1121" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1121" s="3"/>
-    </row>
-    <row r="1122" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1122" s="3"/>
-    </row>
-    <row r="1123" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1123" s="3"/>
-    </row>
-    <row r="1124" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1124" s="3"/>
-    </row>
-    <row r="1125" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1125" s="3"/>
-    </row>
-    <row r="1126" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1126" s="3"/>
-    </row>
-    <row r="1127" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1127" s="3"/>
-    </row>
-    <row r="1128" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1128" s="3"/>
-    </row>
-    <row r="1129" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1129" s="3"/>
-    </row>
-    <row r="1130" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1130" s="3"/>
-    </row>
-    <row r="1131" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1131" s="3"/>
-    </row>
-    <row r="1132" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1132" s="3"/>
-    </row>
-    <row r="1133" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1133" s="3"/>
-    </row>
-    <row r="1134" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1134" s="3"/>
-    </row>
-    <row r="1135" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1135" s="3"/>
-    </row>
-    <row r="1136" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1136" s="3"/>
-    </row>
-    <row r="1137" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1137" s="3"/>
-    </row>
-    <row r="1138" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1138" s="3"/>
-    </row>
-    <row r="1139" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1139" s="3"/>
-    </row>
-    <row r="1140" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1140" s="3"/>
-    </row>
-    <row r="1141" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1141" s="3"/>
-    </row>
-    <row r="1142" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1142" s="3"/>
-    </row>
-    <row r="1143" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1143" s="3"/>
-    </row>
-    <row r="1144" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1144" s="3"/>
-    </row>
-    <row r="1145" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1145" s="3"/>
-    </row>
-    <row r="1146" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1146" s="3"/>
-    </row>
-    <row r="1147" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1147" s="3"/>
-    </row>
-    <row r="1148" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1148" s="3"/>
-    </row>
-    <row r="1149" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1149" s="3"/>
-    </row>
-    <row r="1150" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1150" s="3"/>
-    </row>
-    <row r="1151" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1151" s="3"/>
-    </row>
-    <row r="1152" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1152" s="3"/>
-    </row>
-    <row r="1153" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1153" s="3"/>
-    </row>
-    <row r="1154" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1154" s="3"/>
-    </row>
-    <row r="1155" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1155" s="3"/>
-    </row>
-    <row r="1156" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1156" s="3"/>
-    </row>
-    <row r="1157" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1157" s="3"/>
-    </row>
-    <row r="1158" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1158" s="3"/>
-    </row>
-    <row r="1159" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1159" s="3"/>
-    </row>
-    <row r="1160" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1160" s="3"/>
-    </row>
-    <row r="1161" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1161" s="3"/>
-    </row>
-    <row r="1162" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1162" s="3"/>
-    </row>
-    <row r="1163" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1163" s="3"/>
-    </row>
-    <row r="1164" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1164" s="3"/>
-    </row>
-    <row r="1165" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1165" s="3"/>
-    </row>
-    <row r="1166" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1166" s="3"/>
-    </row>
-    <row r="1167" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1167" s="3"/>
-    </row>
-    <row r="1168" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1168" s="3"/>
-    </row>
-    <row r="1169" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1169" s="3"/>
-    </row>
-    <row r="1170" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1170" s="3"/>
-    </row>
-    <row r="1171" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1171" s="3"/>
-    </row>
-    <row r="1172" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1172" s="3"/>
-    </row>
-    <row r="1173" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1173" s="3"/>
-    </row>
-    <row r="1174" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1174" s="3"/>
-    </row>
-    <row r="1175" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1175" s="3"/>
-    </row>
-    <row r="1176" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1176" s="3"/>
-    </row>
-    <row r="1177" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1177" s="3"/>
-    </row>
-    <row r="1178" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1178" s="3"/>
-    </row>
-    <row r="1179" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1179" s="3"/>
-    </row>
-    <row r="1180" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1180" s="3"/>
-    </row>
-    <row r="1181" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1181" s="3"/>
-    </row>
-    <row r="1182" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1182" s="3"/>
-    </row>
-    <row r="1183" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1183" s="3"/>
-    </row>
-    <row r="1184" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1184" s="3"/>
-    </row>
-    <row r="1185" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1185" s="3"/>
-    </row>
-    <row r="1186" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1186" s="3"/>
-    </row>
-    <row r="1187" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1187" s="3"/>
-    </row>
-    <row r="1188" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1188" s="3"/>
-    </row>
-    <row r="1189" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1189" s="3"/>
-    </row>
-    <row r="1190" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1190" s="3"/>
-    </row>
-    <row r="1191" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1191" s="3"/>
-    </row>
-    <row r="1192" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1192" s="3"/>
-    </row>
-    <row r="1193" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1193" s="3"/>
-    </row>
-    <row r="1194" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1194" s="3"/>
-    </row>
-    <row r="1195" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1195" s="3"/>
-    </row>
-    <row r="1196" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1196" s="3"/>
-    </row>
-    <row r="1197" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1197" s="3"/>
-    </row>
-    <row r="1198" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1198" s="3"/>
-    </row>
-    <row r="1199" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1199" s="3"/>
-    </row>
-    <row r="1200" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1200" s="3"/>
-    </row>
-    <row r="1201" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1201" s="3"/>
-    </row>
-    <row r="1202" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1202" s="3"/>
-    </row>
-    <row r="1203" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1203" s="3"/>
-    </row>
-    <row r="1204" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1204" s="3"/>
-    </row>
-    <row r="1205" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1205" s="3"/>
-    </row>
-    <row r="1206" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1206" s="3"/>
-    </row>
-    <row r="1207" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1207" s="3"/>
-    </row>
-    <row r="1208" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1208" s="3"/>
-    </row>
-    <row r="1209" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1209" s="3"/>
-    </row>
-    <row r="1210" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1210" s="3"/>
-    </row>
-    <row r="1211" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1211" s="3"/>
-    </row>
-    <row r="1212" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1212" s="3"/>
-    </row>
-    <row r="1213" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1213" s="3"/>
-    </row>
-    <row r="1214" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1214" s="3"/>
-    </row>
-    <row r="1215" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1215" s="3"/>
-    </row>
-    <row r="1216" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1216" s="3"/>
-    </row>
-    <row r="1217" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1217" s="3"/>
-    </row>
-    <row r="1218" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1218" s="3"/>
-    </row>
-    <row r="1219" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1219" s="3"/>
-    </row>
-    <row r="1220" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1220" s="3"/>
-    </row>
-    <row r="1221" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1221" s="3"/>
-    </row>
-    <row r="1222" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1222" s="3"/>
-    </row>
-    <row r="1223" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1223" s="3"/>
-    </row>
-    <row r="1224" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1224" s="3"/>
-    </row>
-    <row r="1225" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1225" s="3"/>
-    </row>
-    <row r="1226" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1226" s="3"/>
-    </row>
-    <row r="1227" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1227" s="3"/>
-    </row>
-    <row r="1228" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1228" s="3"/>
-    </row>
-    <row r="1229" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1229" s="3"/>
-    </row>
-    <row r="1230" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1230" s="3"/>
-    </row>
-    <row r="1231" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1231" s="3"/>
-    </row>
-    <row r="1232" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1232" s="3"/>
-    </row>
-    <row r="1233" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1233" s="3"/>
-    </row>
-    <row r="1234" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1234" s="3"/>
-    </row>
-    <row r="1235" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1235" s="3"/>
-    </row>
-    <row r="1236" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1236" s="3"/>
-    </row>
-    <row r="1237" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1237" s="3"/>
-    </row>
-    <row r="1238" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1238" s="3"/>
-    </row>
-    <row r="1239" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1239" s="3"/>
-    </row>
-    <row r="1240" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1240" s="3"/>
-    </row>
-    <row r="1241" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1241" s="3"/>
-    </row>
-    <row r="1242" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1242" s="3"/>
-    </row>
-    <row r="1243" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1243" s="3"/>
-    </row>
-    <row r="1244" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1244" s="3"/>
-    </row>
-    <row r="1245" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1245" s="3"/>
-    </row>
-    <row r="1246" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1246" s="3"/>
-    </row>
-    <row r="1247" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1247" s="3"/>
-    </row>
-    <row r="1248" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1248" s="3"/>
-    </row>
-    <row r="1249" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1249" s="3"/>
-    </row>
-    <row r="1250" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1250" s="3"/>
-    </row>
-    <row r="1251" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1251" s="3"/>
-    </row>
-    <row r="1252" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1252" s="3"/>
-    </row>
-    <row r="1253" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1253" s="3"/>
-    </row>
-    <row r="1254" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1254" s="3"/>
-    </row>
-    <row r="1255" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1255" s="3"/>
-    </row>
-    <row r="1256" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1256" s="3"/>
-    </row>
-    <row r="1257" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1257" s="3"/>
-    </row>
-    <row r="1258" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1258" s="3"/>
-    </row>
-    <row r="1259" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1259" s="3"/>
-    </row>
-    <row r="1260" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1260" s="3"/>
-    </row>
-    <row r="1261" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1261" s="3"/>
-    </row>
-    <row r="1262" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1262" s="3"/>
-    </row>
-    <row r="1263" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1263" s="3"/>
-    </row>
-    <row r="1264" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1264" s="3"/>
-    </row>
-    <row r="1265" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1265" s="3"/>
-    </row>
-    <row r="1266" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1266" s="3"/>
-    </row>
-    <row r="1267" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1267" s="3"/>
-    </row>
-    <row r="1268" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1268" s="3"/>
-    </row>
-    <row r="1269" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1269" s="3"/>
-    </row>
-    <row r="1270" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1270" s="3"/>
-    </row>
-    <row r="1271" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1271" s="3"/>
-    </row>
-    <row r="1272" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1272" s="3"/>
-    </row>
-    <row r="1273" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1273" s="3"/>
-    </row>
-    <row r="1274" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1274" s="3"/>
-    </row>
-    <row r="1275" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1275" s="3"/>
-    </row>
-    <row r="1276" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1276" s="3"/>
-    </row>
-    <row r="1277" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1277" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10966,10 +9385,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:A230"/>
+  <dimension ref="A1:A75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:AO457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11352,161 +9771,6 @@
         <v>673</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11514,10 +9778,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:A371"/>
+  <dimension ref="A1:A216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A217" sqref="A217"/>
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12605,161 +10869,6 @@
         <v>952</v>
       </c>
     </row>
-    <row r="217" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="218" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="219" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="220" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="221" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="222" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="223" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="224" spans="1:1" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>